<commit_message>
Presentation for the experiment added
</commit_message>
<xml_diff>
--- a/comparison_set.xlsx
+++ b/comparison_set.xlsx
@@ -8,13 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivo/VisualStudioProjects/AI4Logistics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2240C698-A1BE-E545-8CE3-6956148794B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A62BB1-D323-CB4F-8179-1B1F08F1403D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="880" windowWidth="25820" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$1:$AD$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$2:$AD$2</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$A$3:$AD$3</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$A$1:$AD$1</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$A$2:$AD$2</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$A$3:$AD$3</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -265,24 +273,23 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$1:$AD$1</c:f>
@@ -480,7 +487,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5AB0-9B49-8549-8B6B744C856B}"/>
@@ -491,17 +497,15 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$1:$AD$1</c:f>
@@ -699,7 +703,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-5AB0-9B49-8549-8B6B744C856B}"/>
@@ -714,10 +717,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
+        <c:gapWidth val="150"/>
         <c:axId val="1829804512"/>
         <c:axId val="1830334160"/>
-      </c:lineChart>
+      </c:barChart>
       <c:catAx>
         <c:axId val="1829804512"/>
         <c:scaling>

</xml_diff>